<commit_message>
changing the project for more security
</commit_message>
<xml_diff>
--- a/combined_participant_data.xlsx
+++ b/combined_participant_data.xlsx
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8758</v>
+        <v>3815</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -463,95 +463,95 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2279</v>
+        <v>3759</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4887</v>
+        <v>3247</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4326</v>
+        <v>8918</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4795</v>
+        <v>2456</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2373</v>
+        <v>8013</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3495</v>
+        <v>8941</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5488</v>
+        <v>1581</v>
       </c>
       <c r="B9" t="n">
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8290</v>
+        <v>5719</v>
       </c>
       <c r="B10" t="n">
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1169</v>
+        <v>7040</v>
       </c>
       <c r="B11" t="n">
         <v>5</v>
@@ -562,18 +562,18 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>8781</v>
+        <v>3315</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4838</v>
+        <v>9821</v>
       </c>
       <c r="B13" t="n">
         <v>2</v>
@@ -584,35 +584,35 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6551</v>
+        <v>6117</v>
       </c>
       <c r="B14" t="n">
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3170</v>
+        <v>6541</v>
       </c>
       <c r="B15" t="n">
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6144</v>
+        <v>5724</v>
       </c>
       <c r="B16" t="n">
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>